<commit_message>
2025-01-22 수요일 오후 03:50
</commit_message>
<xml_diff>
--- a/일잘러/2_엑셀파일다루기/월별구매고객리스트.xlsx
+++ b/일잘러/2_엑셀파일다루기/월별구매고객리스트.xlsx
@@ -1,18 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Documents\파이썬\일잘러\2_엑셀파일다루기\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0D155CD-4C46-4427-9ACD-E17874BB5813}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="10월"/>
-    <sheet r:id="rId2" sheetId="2" name="11월"/>
-    <sheet r:id="rId3" sheetId="3" name="12월"/>
-    <sheet r:id="rId4" sheetId="4" name="2023년_전체"/>
+    <sheet name="10월" sheetId="1" r:id="rId1"/>
+    <sheet name="11월" sheetId="2" r:id="rId2"/>
+    <sheet name="12월" sheetId="3" r:id="rId3"/>
+    <sheet name="2023년_전체" sheetId="4" r:id="rId4"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -169,15 +186,15 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm월 dd일"/>
+    <numFmt numFmtId="176" formatCode="mm&quot;월&quot;\ dd&quot;일&quot;"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="맑은 고딕"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -186,6 +203,13 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -216,40 +240,35 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="표준" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -260,10 +279,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -301,71 +320,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -393,7 +412,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -416,11 +435,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -429,13 +448,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -445,7 +464,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -454,7 +473,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -463,7 +482,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -471,10 +490,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -539,7 +558,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -547,19 +566,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="9.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="20.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="12.290714285714287" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>48</v>
       </c>
@@ -571,7 +588,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -597,7 +614,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45202</v>
       </c>
@@ -621,9 +638,10 @@
       </c>
       <c r="H3" s="5">
         <f>C3*G3</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45215</v>
       </c>
@@ -647,9 +665,10 @@
       </c>
       <c r="H4" s="5">
         <f>C4*G4</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45221</v>
       </c>
@@ -673,9 +692,10 @@
       </c>
       <c r="H5" s="5">
         <f>C5*G5</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45228</v>
       </c>
@@ -699,9 +719,10 @@
       </c>
       <c r="H6" s="5">
         <f>C6*G6</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>144000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45228</v>
       </c>
@@ -725,15 +746,17 @@
       </c>
       <c r="H7" s="5">
         <f>C7*G7</f>
+        <v>136000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -741,19 +764,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>47</v>
       </c>
@@ -765,7 +785,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -791,7 +811,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45231</v>
       </c>
@@ -815,9 +835,10 @@
       </c>
       <c r="H3" s="5">
         <f>C3*G9</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45234</v>
       </c>
@@ -840,10 +861,11 @@
         <v>18000</v>
       </c>
       <c r="H4" s="5">
-        <f>C4*G4</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <f t="shared" ref="H4:H10" si="0">C4*G4</f>
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45241</v>
       </c>
@@ -866,10 +888,11 @@
         <v>36000</v>
       </c>
       <c r="H5" s="5">
-        <f>C5*G5</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45242</v>
       </c>
@@ -892,10 +915,11 @@
         <v>36000</v>
       </c>
       <c r="H6" s="5">
-        <f>C6*G6</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45246</v>
       </c>
@@ -918,10 +942,11 @@
         <v>36000</v>
       </c>
       <c r="H7" s="5">
-        <f>C7*G7</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>45255</v>
       </c>
@@ -944,10 +969,11 @@
         <v>18000</v>
       </c>
       <c r="H8" s="5">
-        <f>C8*G8</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45258</v>
       </c>
@@ -970,10 +996,11 @@
         <v>20000</v>
       </c>
       <c r="H9" s="5">
-        <f>C9*G9</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45260</v>
       </c>
@@ -996,36 +1023,39 @@
         <v>20000</v>
       </c>
       <c r="H10" s="5">
-        <f>C10*G10</f>
+        <f t="shared" si="0"/>
+        <v>40000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="9.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="20.290714285714284" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="9.875" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.25" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>46</v>
       </c>
@@ -1037,7 +1067,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1063,7 +1093,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45273</v>
       </c>
@@ -1087,9 +1117,10 @@
       </c>
       <c r="H3" s="5">
         <f>C3*G3</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45277</v>
       </c>
@@ -1113,9 +1144,10 @@
       </c>
       <c r="H4" s="5">
         <f>C4*G4</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45282</v>
       </c>
@@ -1139,9 +1171,10 @@
       </c>
       <c r="H5" s="5">
         <f>C5*G5</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45287</v>
       </c>
@@ -1165,15 +1198,18 @@
       </c>
       <c r="H6" s="5">
         <f>C6*G6</f>
+        <v>80000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -1181,19 +1217,16 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" style="6" width="12.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="7" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="8" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="12.625" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="13.625" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="13.625" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1205,7 +1238,7 @@
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1231,7 +1264,7 @@
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>45202</v>
       </c>
@@ -1255,9 +1288,10 @@
       </c>
       <c r="H3" s="5">
         <f>C3*G3</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="4">
         <v>45215</v>
       </c>
@@ -1281,9 +1315,10 @@
       </c>
       <c r="H4" s="5">
         <f>C4*G4</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="4">
         <v>45221</v>
       </c>
@@ -1307,9 +1342,10 @@
       </c>
       <c r="H5" s="5">
         <f>C5*G5</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4">
         <v>45228</v>
       </c>
@@ -1333,9 +1369,10 @@
       </c>
       <c r="H6" s="5">
         <f>C6*G6</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+        <v>144000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>45228</v>
       </c>
@@ -1359,9 +1396,10 @@
       </c>
       <c r="H7" s="5">
         <f>C7*G7</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+        <v>136000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>45231</v>
       </c>
@@ -1385,9 +1423,10 @@
       </c>
       <c r="H8" s="5">
         <f>C8*G14</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+        <v>60000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>45234</v>
       </c>
@@ -1410,10 +1449,11 @@
         <v>18000</v>
       </c>
       <c r="H9" s="5">
-        <f>C9*G9</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+        <f t="shared" ref="H9:H19" si="0">C9*G9</f>
+        <v>54000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="4">
         <v>45241</v>
       </c>
@@ -1436,10 +1476,11 @@
         <v>36000</v>
       </c>
       <c r="H10" s="5">
-        <f>C10*G10</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>45242</v>
       </c>
@@ -1462,10 +1503,11 @@
         <v>36000</v>
       </c>
       <c r="H11" s="5">
-        <f>C11*G11</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>45246</v>
       </c>
@@ -1488,10 +1530,11 @@
         <v>36000</v>
       </c>
       <c r="H12" s="5">
-        <f>C12*G12</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>45255</v>
       </c>
@@ -1514,10 +1557,11 @@
         <v>18000</v>
       </c>
       <c r="H13" s="5">
-        <f>C13*G13</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>45258</v>
       </c>
@@ -1540,10 +1584,11 @@
         <v>20000</v>
       </c>
       <c r="H14" s="5">
-        <f>C14*G14</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="4">
         <v>45260</v>
       </c>
@@ -1566,10 +1611,11 @@
         <v>20000</v>
       </c>
       <c r="H15" s="5">
-        <f>C15*G15</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>45273</v>
       </c>
@@ -1592,10 +1638,11 @@
         <v>36000</v>
       </c>
       <c r="H16" s="5">
-        <f>C16*G16</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>72000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>45277</v>
       </c>
@@ -1618,10 +1665,11 @@
         <v>36000</v>
       </c>
       <c r="H17" s="5">
-        <f>C17*G17</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>36000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>45282</v>
       </c>
@@ -1644,10 +1692,11 @@
         <v>18000</v>
       </c>
       <c r="H18" s="5">
-        <f>C18*G18</f>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+        <f t="shared" si="0"/>
+        <v>18000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
         <v>45287</v>
       </c>
@@ -1670,10 +1719,12 @@
         <v>20000</v>
       </c>
       <c r="H19" s="5">
-        <f>C19*G19</f>
+        <f t="shared" si="0"/>
+        <v>80000</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>